<commit_message>
Update host_port configuration for local testing and enhance feedback extraction logic in grading response
</commit_message>
<xml_diff>
--- a/ela_rag_docker/test_scripts/question_list_with_all_essays.xlsx
+++ b/ela_rag_docker/test_scripts/question_list_with_all_essays.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://psypheritcomau-my.sharepoint.com/personal/hayden_logical-aspect_com_au/Documents/Education/UniSA/INFT3039 - Capstone 1/ela_rag_docker/test_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{56FA64AA-56CA-4594-BB3D-0BB7E2F4B3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5D86008-411F-4A36-876E-CA7860340B31}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{56FA64AA-56CA-4594-BB3D-0BB7E2F4B3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1DC6960-1A5D-4245-B491-C4EC7E1AFFA1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3266,10 +3266,14 @@
   <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="134.85546875" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5462,5 +5466,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>